<commit_message>
Revision for IAEA meeting
</commit_message>
<xml_diff>
--- a/data_export.xlsx
+++ b/data_export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Net-Zero Scenario</t>
+  </si>
+  <si>
+    <t>Cogeneration Scenario</t>
+  </si>
+  <si>
+    <t>Demand Efficiency Scenario</t>
+  </si>
+  <si>
+    <t>Low Demand Scenario</t>
+  </si>
+  <si>
+    <t>No-Nuclear Scenario</t>
   </si>
   <si>
     <t>CO2 Scenario</t>
@@ -624,14 +636,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
@@ -694,16 +706,16 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H2">
         <v>293.826</v>
@@ -726,16 +738,16 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H3">
         <v>4.831633921824</v>
@@ -758,16 +770,16 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H4">
         <v>293.363</v>
@@ -790,16 +802,16 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H5">
         <v>5.10690013704</v>
@@ -822,16 +834,16 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H6">
         <v>301.963</v>
@@ -854,16 +866,16 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H7">
         <v>4.939373461680001</v>
@@ -886,16 +898,16 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H8">
         <v>301.468</v>
@@ -918,16 +930,16 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H9">
         <v>4.93035114384</v>
@@ -950,16 +962,16 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H10">
         <v>311.957</v>
@@ -982,16 +994,16 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H11">
         <v>5.369323671360001</v>
@@ -1014,16 +1026,16 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H12">
         <v>310.143</v>
@@ -1046,16 +1058,16 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H13">
         <v>5.32106263368</v>
@@ -1078,16 +1090,16 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H14">
         <v>397.9</v>
@@ -1107,16 +1119,16 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I15">
         <v>1.656</v>
@@ -1136,16 +1148,16 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K16">
         <v>0.135</v>
@@ -1159,16 +1171,16 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H17">
         <v>397.2</v>
@@ -1188,16 +1200,16 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K18">
         <v>0.036</v>
@@ -1211,16 +1223,16 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I19">
         <v>0.5850000000000001</v>
@@ -1237,16 +1249,16 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I20">
         <v>0.261</v>
@@ -1263,16 +1275,16 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="I21">
         <v>0.324</v>
@@ -1289,16 +1301,16 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G22">
         <v>349.81</v>
@@ -1315,16 +1327,16 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G23">
         <v>4.312404</v>
@@ -1341,16 +1353,16 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G24">
         <v>0.167472</v>
@@ -1367,16 +1379,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G25">
         <v>0.018</v>
@@ -1393,16 +1405,16 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G26">
         <v>0.879228</v>
@@ -1419,16 +1431,16 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G27">
         <v>0.544284</v>
@@ -1445,16 +1457,16 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G28">
         <v>1.758456</v>
@@ -1471,16 +1483,16 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G29">
         <v>0.3636</v>
@@ -1497,16 +1509,16 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G30">
         <v>1.46538</v>
@@ -1523,16 +1535,16 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G31">
         <v>0.083736</v>
@@ -1549,16 +1561,16 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G32">
         <v>0.334944</v>
@@ -1575,16 +1587,16 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G33">
         <v>0.293076</v>
@@ -1601,16 +1613,16 @@
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G34">
         <v>1.214172</v>
@@ -1627,16 +1639,16 @@
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G35">
         <v>0.3384</v>
@@ -1653,16 +1665,16 @@
         <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G36">
         <v>1.0467</v>
@@ -1679,16 +1691,16 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G37">
         <v>0.8373600000000001</v>
@@ -1705,16 +1717,16 @@
         <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F38" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G38">
         <v>0.007200000000000001</v>
@@ -1731,16 +1743,16 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E39" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G39">
         <v>1.5826104</v>
@@ -1757,16 +1769,16 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F40" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G40">
         <v>0.167472</v>
@@ -1783,16 +1795,16 @@
         <v>24</v>
       </c>
       <c r="C41" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G41">
         <v>0.9755244000000001</v>
@@ -1809,16 +1821,16 @@
         <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G42">
         <v>0.0083736</v>
@@ -1835,16 +1847,16 @@
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E43" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G43">
         <v>0.0167472</v>
@@ -1861,16 +1873,16 @@
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G44">
         <v>0.083736</v>
@@ -1887,16 +1899,16 @@
         <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G45">
         <v>0.20934</v>
@@ -1913,16 +1925,16 @@
         <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H46">
         <v>0.334944</v>
@@ -1936,16 +1948,16 @@
         <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G47">
         <v>0.083736</v>
@@ -1962,16 +1974,16 @@
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E48" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F48" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G48">
         <v>0.020934</v>
@@ -1988,16 +2000,16 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F49" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G49">
         <v>0.0167472</v>
@@ -2014,16 +2026,16 @@
         <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D50" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E50" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F50" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G50">
         <v>0.8712000000000001</v>
@@ -2040,16 +2052,16 @@
         <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E51" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F51" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G51">
         <v>0.2376</v>
@@ -2066,16 +2078,16 @@
         <v>24</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E52" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F52" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G52">
         <v>0.3852</v>
@@ -2092,16 +2104,16 @@
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F53" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H53">
         <v>0.1152</v>
@@ -2115,16 +2127,16 @@
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F54" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G54">
         <v>0.0252</v>
@@ -2141,16 +2153,16 @@
         <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G55">
         <v>0.2232</v>
@@ -2161,109 +2173,106 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D56" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E56" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="G56">
+        <v>352.73</v>
       </c>
       <c r="H56">
-        <v>673</v>
-      </c>
-      <c r="I56">
-        <v>1175</v>
+        <v>579.729</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E57" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F57" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="G57">
+        <v>332.73</v>
       </c>
       <c r="H57">
-        <v>466.9</v>
-      </c>
-      <c r="I57">
-        <v>695</v>
+        <v>516.73</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D58" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F58" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="G58">
+        <v>328.09</v>
       </c>
       <c r="H58">
-        <v>4.417074</v>
-      </c>
-      <c r="I58">
-        <v>5.8447728</v>
-      </c>
-      <c r="L58">
-        <v>6.866352</v>
+        <v>502.8135</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F59" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="G59">
+        <v>355.74</v>
       </c>
       <c r="H59">
-        <v>0.6866352</v>
-      </c>
-      <c r="I59">
-        <v>0.8666676</v>
+        <v>585.76</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -2271,28 +2280,25 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D60" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E60" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F60" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H60">
-        <v>0.962964</v>
+        <v>531.67</v>
       </c>
       <c r="I60">
-        <v>1.381644</v>
-      </c>
-      <c r="L60">
-        <v>3.8183616</v>
+        <v>928.25</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -2300,22 +2306,25 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E61" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F61" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H61">
+        <v>368.851</v>
       </c>
       <c r="I61">
-        <v>1.4109516</v>
+        <v>549.05</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -2323,22 +2332,28 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D62" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="E62" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H62">
+        <v>4.417074</v>
       </c>
       <c r="I62">
-        <v>0.1632852</v>
+        <v>5.8447728</v>
+      </c>
+      <c r="L62">
+        <v>6.866352</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -2346,25 +2361,25 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="E63" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F63" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H63">
+        <v>0.6866352</v>
       </c>
       <c r="I63">
-        <v>0.02736</v>
-      </c>
-      <c r="L63">
-        <v>0.8910000000000001</v>
+        <v>0.8666676</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -2372,25 +2387,28 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D64" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E64" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F64" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H64">
-        <v>1.5198084</v>
+        <v>0.962964</v>
       </c>
       <c r="I64">
-        <v>2.1813228</v>
+        <v>1.381644</v>
+      </c>
+      <c r="L64">
+        <v>3.8183616</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -2398,25 +2416,22 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D65" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F65" t="s">
-        <v>79</v>
-      </c>
-      <c r="H65">
-        <v>0.4320000000000001</v>
+        <v>83</v>
       </c>
       <c r="I65">
-        <v>0.6519600000000001</v>
+        <v>1.4109516</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -2424,22 +2439,22 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D66" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E66" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F66" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I66">
-        <v>1.904994</v>
+        <v>0.1632852</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -2447,22 +2462,25 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D67" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E67" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F67" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I67">
-        <v>0.293076</v>
+        <v>0.02736</v>
+      </c>
+      <c r="L67">
+        <v>0.8910000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -2470,25 +2488,25 @@
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D68" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E68" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F68" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H68">
-        <v>1.0801944</v>
+        <v>1.5198084</v>
       </c>
       <c r="I68">
-        <v>1.235106</v>
+        <v>2.1813228</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -2496,25 +2514,25 @@
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E69" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F69" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H69">
-        <v>0.21852</v>
+        <v>0.4320000000000001</v>
       </c>
       <c r="I69">
-        <v>0.29916</v>
+        <v>0.6519600000000001</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -2522,25 +2540,22 @@
         <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C70" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D70" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E70" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F70" t="s">
-        <v>79</v>
-      </c>
-      <c r="H70">
-        <v>0.29016</v>
+        <v>83</v>
       </c>
       <c r="I70">
-        <v>0.4122</v>
+        <v>1.904994</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -2548,22 +2563,22 @@
         <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D71" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E71" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F71" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I71">
-        <v>0.690822</v>
+        <v>0.293076</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -2571,25 +2586,25 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E72" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F72" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H72">
-        <v>1.130436</v>
+        <v>1.0801944</v>
       </c>
       <c r="I72">
-        <v>1.5616764</v>
+        <v>1.235106</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -2597,25 +2612,25 @@
         <v>16</v>
       </c>
       <c r="B73" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D73" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E73" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F73" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H73">
-        <v>0.00504</v>
+        <v>0.21852</v>
       </c>
       <c r="I73">
-        <v>0.0306</v>
+        <v>0.29916</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -2623,28 +2638,25 @@
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D74" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="E74" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H74">
-        <v>6.1629696</v>
+        <v>0.29016</v>
       </c>
       <c r="I74">
-        <v>8.331732000000001</v>
-      </c>
-      <c r="L74">
-        <v>10.467</v>
+        <v>0.4122</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -2652,28 +2664,22 @@
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C75" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D75" t="s">
         <v>54</v>
       </c>
       <c r="E75" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F75" t="s">
-        <v>79</v>
-      </c>
-      <c r="H75">
-        <v>1.6998408</v>
+        <v>83</v>
       </c>
       <c r="I75">
-        <v>2.0054772</v>
-      </c>
-      <c r="L75">
-        <v>0.376812</v>
+        <v>0.690822</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -2681,28 +2687,25 @@
         <v>16</v>
       </c>
       <c r="B76" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D76" t="s">
         <v>55</v>
       </c>
       <c r="E76" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F76" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H76">
-        <v>1.6663464</v>
+        <v>1.130436</v>
       </c>
       <c r="I76">
-        <v>1.9971036</v>
-      </c>
-      <c r="L76">
-        <v>1.2267324</v>
+        <v>1.5616764</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -2710,25 +2713,25 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D77" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E77" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F77" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H77">
+        <v>0.00504</v>
       </c>
       <c r="I77">
-        <v>0.334944</v>
-      </c>
-      <c r="L77">
-        <v>3.0689244</v>
+        <v>0.0306</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -2736,28 +2739,28 @@
         <v>16</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C78" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D78" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E78" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F78" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H78">
-        <v>1.7668296</v>
+        <v>6.1629696</v>
       </c>
       <c r="I78">
-        <v>2.2943664</v>
+        <v>8.331732000000001</v>
       </c>
       <c r="L78">
-        <v>0.586152</v>
+        <v>10.467</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -2765,28 +2768,28 @@
         <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C79" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E79" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F79" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H79">
-        <v>1.0299528</v>
+        <v>1.6998408</v>
       </c>
       <c r="I79">
-        <v>1.6998408</v>
+        <v>2.0054772</v>
       </c>
       <c r="L79">
-        <v>5.2335</v>
+        <v>0.376812</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -2794,347 +2797,320 @@
         <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D80" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E80" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F80" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H80">
-        <v>1.10412</v>
+        <v>1.6663464</v>
       </c>
       <c r="I80">
-        <v>1.62972</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11">
+        <v>1.9971036</v>
+      </c>
+      <c r="L80">
+        <v>1.2267324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C81" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D81" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E81" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F81" t="s">
-        <v>79</v>
-      </c>
-      <c r="H81">
-        <v>0.63612</v>
+        <v>83</v>
       </c>
       <c r="I81">
-        <v>0.7243200000000001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11">
+        <v>0.334944</v>
+      </c>
+      <c r="L81">
+        <v>3.0689244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>16</v>
       </c>
       <c r="B82" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C82" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D82" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E82" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F82" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H82">
-        <v>0.28116</v>
+        <v>1.7668296</v>
       </c>
       <c r="I82">
-        <v>0.3164400000000001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11">
+        <v>2.2943664</v>
+      </c>
+      <c r="L82">
+        <v>0.586152</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>16</v>
       </c>
       <c r="B83" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C83" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D83" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E83" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F83" t="s">
-        <v>79</v>
+        <v>83</v>
+      </c>
+      <c r="H83">
+        <v>1.0299528</v>
       </c>
       <c r="I83">
-        <v>0.13392</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11">
+        <v>1.6998408</v>
+      </c>
+      <c r="L83">
+        <v>5.2335</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D84" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E84" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F84" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H84">
-        <v>0.05796000000000001</v>
+        <v>1.10412</v>
       </c>
       <c r="I84">
-        <v>0.0738</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11">
+        <v>1.62972</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C85" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D85" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E85" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F85" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H85">
-        <v>0.468</v>
+        <v>0.63612</v>
       </c>
       <c r="I85">
-        <v>0.7714800000000002</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11">
+        <v>0.7243200000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D86" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E86" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F86" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H86">
-        <v>0.0396</v>
+        <v>0.28116</v>
       </c>
       <c r="I86">
-        <v>0.18792</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11">
+        <v>0.3164400000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D87" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E87" t="s">
+        <v>82</v>
+      </c>
+      <c r="F87" t="s">
+        <v>83</v>
+      </c>
+      <c r="I87">
+        <v>0.13392</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C88" t="s">
+        <v>33</v>
+      </c>
+      <c r="D88" t="s">
         <v>78</v>
       </c>
-      <c r="F87" t="s">
-        <v>79</v>
-      </c>
-      <c r="H87">
-        <v>0.08928000000000001</v>
-      </c>
-      <c r="I87">
-        <v>0.19332</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11">
-      <c r="A88" t="s">
-        <v>17</v>
-      </c>
-      <c r="B88" t="s">
-        <v>24</v>
-      </c>
-      <c r="C88" t="s">
-        <v>29</v>
-      </c>
-      <c r="D88" t="s">
-        <v>38</v>
-      </c>
       <c r="E88" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F88" t="s">
-        <v>82</v>
-      </c>
-      <c r="G88">
-        <v>3.491791200000001</v>
+        <v>83</v>
       </c>
       <c r="H88">
-        <v>5.057654400000001</v>
+        <v>0.05796000000000001</v>
       </c>
       <c r="I88">
-        <v>7.661844</v>
-      </c>
-      <c r="J88">
-        <v>11.7146664</v>
-      </c>
-      <c r="K88">
-        <v>17.9864928</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11">
+        <v>0.0738</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C89" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
         <v>39</v>
       </c>
       <c r="E89" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F89" t="s">
-        <v>82</v>
-      </c>
-      <c r="G89">
-        <v>0.2135268</v>
+        <v>83</v>
       </c>
       <c r="H89">
-        <v>0.3181968</v>
+        <v>0.468</v>
       </c>
       <c r="I89">
-        <v>0.4940424</v>
-      </c>
-      <c r="J89">
-        <v>0.7619976000000001</v>
-      </c>
-      <c r="K89">
-        <v>1.1806776</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11">
+        <v>0.7714800000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B90" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C90" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D90" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="E90" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F90" t="s">
-        <v>82</v>
-      </c>
-      <c r="G90">
-        <v>1.2811608</v>
+        <v>83</v>
       </c>
       <c r="H90">
-        <v>1.925928</v>
+        <v>0.0396</v>
       </c>
       <c r="I90">
-        <v>2.972628</v>
-      </c>
-      <c r="J90">
-        <v>4.5929196</v>
-      </c>
-      <c r="K90">
-        <v>7.096626000000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11">
+        <v>0.18792</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D91" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="E91" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F91" t="s">
-        <v>82</v>
-      </c>
-      <c r="G91">
-        <v>0.146538</v>
+        <v>83</v>
       </c>
       <c r="H91">
-        <v>0.2177136</v>
+        <v>0.08928000000000001</v>
       </c>
       <c r="I91">
-        <v>0.334944</v>
-      </c>
-      <c r="J91">
-        <v>0.5191632</v>
-      </c>
-      <c r="K91">
-        <v>0.7996788000000001</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11">
+        <v>0.19332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -3142,34 +3118,34 @@
         <v>24</v>
       </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D92" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E92" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F92" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G92">
-        <v>1.2099852</v>
+        <v>3.491791200000001</v>
       </c>
       <c r="H92">
-        <v>1.632852</v>
+        <v>5.057654400000001</v>
       </c>
       <c r="I92">
-        <v>2.3697288</v>
+        <v>7.661844</v>
       </c>
       <c r="J92">
-        <v>3.5420328</v>
+        <v>11.7146664</v>
       </c>
       <c r="K92">
-        <v>5.354917200000001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11">
+        <v>17.9864928</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -3177,136 +3153,136 @@
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D93" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F93" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G93">
-        <v>0.6405804</v>
+        <v>0.2135268</v>
       </c>
       <c r="H93">
-        <v>0.962964</v>
+        <v>0.3181968</v>
       </c>
       <c r="I93">
-        <v>1.486314</v>
+        <v>0.4940424</v>
       </c>
       <c r="J93">
-        <v>2.2985532</v>
+        <v>0.7619976000000001</v>
       </c>
       <c r="K93">
-        <v>3.5504064</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11">
+        <v>1.1806776</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C94" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E94" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F94" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G94">
-        <v>3.491791200000001</v>
+        <v>1.2811608</v>
       </c>
       <c r="H94">
-        <v>4.571985600000001</v>
+        <v>1.925928</v>
       </c>
       <c r="I94">
-        <v>6.9961428</v>
+        <v>2.972628</v>
       </c>
       <c r="J94">
-        <v>11.0489652</v>
+        <v>4.5929196</v>
       </c>
       <c r="K94">
-        <v>17.3207916</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11">
+        <v>7.096626000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C95" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D95" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E95" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F95" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G95">
-        <v>0.2135268</v>
+        <v>0.146538</v>
       </c>
       <c r="H95">
-        <v>0.3181968</v>
+        <v>0.2177136</v>
       </c>
       <c r="I95">
-        <v>0.4940424</v>
+        <v>0.334944</v>
       </c>
       <c r="J95">
-        <v>0.7619976000000001</v>
+        <v>0.5191632</v>
       </c>
       <c r="K95">
-        <v>1.1806776</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11">
+        <v>0.7996788000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>17</v>
       </c>
       <c r="B96" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D96" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E96" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F96" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G96">
-        <v>1.2811608</v>
+        <v>1.2099852</v>
       </c>
       <c r="H96">
-        <v>1.7124012</v>
+        <v>1.632852</v>
       </c>
       <c r="I96">
-        <v>2.7172332</v>
+        <v>2.3697288</v>
       </c>
       <c r="J96">
-        <v>4.3375248</v>
+        <v>3.5420328</v>
       </c>
       <c r="K96">
-        <v>6.841231200000001</v>
+        <v>5.354917200000001</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -3314,34 +3290,34 @@
         <v>17</v>
       </c>
       <c r="B97" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D97" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E97" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F97" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G97">
-        <v>0.146538</v>
+        <v>0.6405804</v>
       </c>
       <c r="H97">
-        <v>0.2177136</v>
+        <v>0.962964</v>
       </c>
       <c r="I97">
-        <v>0.334944</v>
+        <v>1.486314</v>
       </c>
       <c r="J97">
-        <v>0.5191632</v>
+        <v>2.2985532</v>
       </c>
       <c r="K97">
-        <v>0.7996788000000001</v>
+        <v>3.5504064</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -3349,34 +3325,34 @@
         <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C98" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D98" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E98" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F98" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G98">
-        <v>1.2099852</v>
+        <v>3.491791200000001</v>
       </c>
       <c r="H98">
-        <v>1.3942044</v>
+        <v>4.571985600000001</v>
       </c>
       <c r="I98">
-        <v>2.009664</v>
+        <v>6.9961428</v>
       </c>
       <c r="J98">
-        <v>3.177781200000001</v>
+        <v>11.0489652</v>
       </c>
       <c r="K98">
-        <v>4.9948524</v>
+        <v>17.3207916</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -3384,34 +3360,34 @@
         <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D99" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E99" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F99" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G99">
-        <v>0.6405804</v>
+        <v>0.2135268</v>
       </c>
       <c r="H99">
-        <v>0.9294696</v>
+        <v>0.3181968</v>
       </c>
       <c r="I99">
-        <v>1.444446</v>
+        <v>0.4940424</v>
       </c>
       <c r="J99">
-        <v>2.2524984</v>
+        <v>0.7619976000000001</v>
       </c>
       <c r="K99">
-        <v>3.5043516</v>
+        <v>1.1806776</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -3419,34 +3395,34 @@
         <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D100" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E100" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F100" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G100">
-        <v>3.491791200000001</v>
+        <v>1.2811608</v>
       </c>
       <c r="H100">
-        <v>4.810633200000001</v>
+        <v>1.7124012</v>
       </c>
       <c r="I100">
-        <v>7.305966000000001</v>
+        <v>2.7172332</v>
       </c>
       <c r="J100">
-        <v>11.3587884</v>
+        <v>4.3375248</v>
       </c>
       <c r="K100">
-        <v>17.6306148</v>
+        <v>6.841231200000001</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -3454,34 +3430,34 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E101" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F101" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G101">
-        <v>0.2135268</v>
+        <v>0.146538</v>
       </c>
       <c r="H101">
-        <v>0.3181968</v>
+        <v>0.2177136</v>
       </c>
       <c r="I101">
-        <v>0.4940424</v>
+        <v>0.334944</v>
       </c>
       <c r="J101">
-        <v>0.7619976000000001</v>
+        <v>0.5191632</v>
       </c>
       <c r="K101">
-        <v>1.1806776</v>
+        <v>0.7996788000000001</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -3489,34 +3465,34 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D102" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E102" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F102" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G102">
-        <v>1.2811608</v>
+        <v>1.2099852</v>
       </c>
       <c r="H102">
-        <v>1.8170712</v>
+        <v>1.3942044</v>
       </c>
       <c r="I102">
-        <v>2.8428372</v>
+        <v>2.009664</v>
       </c>
       <c r="J102">
-        <v>4.4631288</v>
+        <v>3.177781200000001</v>
       </c>
       <c r="K102">
-        <v>6.9668352</v>
+        <v>4.9948524</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -3524,34 +3500,34 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D103" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E103" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F103" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G103">
-        <v>0.146538</v>
+        <v>0.6405804</v>
       </c>
       <c r="H103">
-        <v>0.2177136</v>
+        <v>0.9294696</v>
       </c>
       <c r="I103">
-        <v>0.334944</v>
+        <v>1.444446</v>
       </c>
       <c r="J103">
-        <v>0.5191632</v>
+        <v>2.2524984</v>
       </c>
       <c r="K103">
-        <v>0.7996788000000001</v>
+        <v>3.5043516</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -3559,34 +3535,34 @@
         <v>17</v>
       </c>
       <c r="B104" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C104" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D104" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E104" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F104" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G104">
-        <v>1.2099852</v>
+        <v>3.491791200000001</v>
       </c>
       <c r="H104">
-        <v>1.5114348</v>
+        <v>4.810633200000001</v>
       </c>
       <c r="I104">
-        <v>2.1896964</v>
+        <v>7.305966000000001</v>
       </c>
       <c r="J104">
-        <v>3.357813600000001</v>
+        <v>11.3587884</v>
       </c>
       <c r="K104">
-        <v>5.1748848</v>
+        <v>17.6306148</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -3594,33 +3570,173 @@
         <v>17</v>
       </c>
       <c r="B105" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C105" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D105" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E105" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F105" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G105">
+        <v>0.2135268</v>
+      </c>
+      <c r="H105">
+        <v>0.3181968</v>
+      </c>
+      <c r="I105">
+        <v>0.4940424</v>
+      </c>
+      <c r="J105">
+        <v>0.7619976000000001</v>
+      </c>
+      <c r="K105">
+        <v>1.1806776</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="A106" t="s">
+        <v>17</v>
+      </c>
+      <c r="B106" t="s">
+        <v>32</v>
+      </c>
+      <c r="C106" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" t="s">
+        <v>82</v>
+      </c>
+      <c r="F106" t="s">
+        <v>86</v>
+      </c>
+      <c r="G106">
+        <v>1.2811608</v>
+      </c>
+      <c r="H106">
+        <v>1.8170712</v>
+      </c>
+      <c r="I106">
+        <v>2.8428372</v>
+      </c>
+      <c r="J106">
+        <v>4.4631288</v>
+      </c>
+      <c r="K106">
+        <v>6.9668352</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="A107" t="s">
+        <v>17</v>
+      </c>
+      <c r="B107" t="s">
+        <v>32</v>
+      </c>
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" t="s">
+        <v>82</v>
+      </c>
+      <c r="F107" t="s">
+        <v>86</v>
+      </c>
+      <c r="G107">
+        <v>0.146538</v>
+      </c>
+      <c r="H107">
+        <v>0.2177136</v>
+      </c>
+      <c r="I107">
+        <v>0.334944</v>
+      </c>
+      <c r="J107">
+        <v>0.5191632</v>
+      </c>
+      <c r="K107">
+        <v>0.7996788000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="A108" t="s">
+        <v>17</v>
+      </c>
+      <c r="B108" t="s">
+        <v>32</v>
+      </c>
+      <c r="C108" t="s">
+        <v>33</v>
+      </c>
+      <c r="D108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" t="s">
+        <v>82</v>
+      </c>
+      <c r="F108" t="s">
+        <v>86</v>
+      </c>
+      <c r="G108">
+        <v>1.2099852</v>
+      </c>
+      <c r="H108">
+        <v>1.5114348</v>
+      </c>
+      <c r="I108">
+        <v>2.1896964</v>
+      </c>
+      <c r="J108">
+        <v>3.357813600000001</v>
+      </c>
+      <c r="K108">
+        <v>5.1748848</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="A109" t="s">
+        <v>17</v>
+      </c>
+      <c r="B109" t="s">
+        <v>32</v>
+      </c>
+      <c r="C109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D109" t="s">
+        <v>55</v>
+      </c>
+      <c r="E109" t="s">
+        <v>82</v>
+      </c>
+      <c r="F109" t="s">
+        <v>86</v>
+      </c>
+      <c r="G109">
         <v>0.6405804</v>
       </c>
-      <c r="H105">
+      <c r="H109">
         <v>0.94203</v>
       </c>
-      <c r="I105">
+      <c r="I109">
         <v>1.444446</v>
       </c>
-      <c r="J105">
+      <c r="J109">
         <v>2.2524984</v>
       </c>
-      <c r="K105">
+      <c r="K109">
         <v>3.5043516</v>
       </c>
     </row>
@@ -3631,14 +3747,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3650,7 +3766,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3683,7 +3799,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3694,7 +3810,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -3705,7 +3821,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -3716,7 +3832,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -3727,7 +3843,7 @@
         <v>24</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -3754,21 +3870,21 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -3776,10 +3892,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -3787,10 +3903,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -3798,12 +3914,56 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="b">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>